<commit_message>
Tested for ThermalUnitBlock and set on dimensions
- Network taken from Excel (useful in test phase)
- Trasnformation of generators in dictionaries ready to be read (still to test on the other components, similar approach)
- Still to add documentation
</commit_message>
<xml_diff>
--- a/data/microgrid/components.xlsx
+++ b/data/microgrid/components.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>solar</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>wind</t>
+  </si>
+  <si>
+    <t>p_max_pu</t>
+  </si>
+  <si>
+    <t>diesel</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,10 +647,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,10 +660,11 @@
     <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -673,8 +680,11 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -689,6 +699,26 @@
       </c>
       <c r="E2" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>